<commit_message>
resolving cell issues for creation of columns
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59,12 +69,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Column Creation on basic JSON completed
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>fruit</t>
+  </si>
   <si>
     <t>size</t>
   </si>
@@ -69,13 +72,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -85,6 +88,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>